<commit_message>
[Master] [模組名稱：Drink Order] [功能名稱：Drink Order]  
1. API SaveDrinksOrder 出版
2. API DrinksOrderList 出版
</commit_message>
<xml_diff>
--- a/Document/飲料訂單_TableSchema.xlsx
+++ b/Document/飲料訂單_TableSchema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_WorkSpace\GitWorkSpace\GitProject\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF83E6C-9413-4A60-94F0-9CD274826D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AA84F0-5A41-478A-9A82-A54F82B4A6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1272" yWindow="0" windowWidth="21768" windowHeight="12360" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="基礎表" sheetId="3" r:id="rId1"/>
@@ -4635,7 +4635,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4773,6 +4773,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文件" ma:contentTypeID="0x010100794E18DF04B3B54DA3827C6951F00E0A" ma:contentTypeVersion="0" ma:contentTypeDescription="建立新的文件。" ma:contentTypeScope="" ma:versionID="ce9216499caa1e3b8d20922f0be76bb4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2f2c8fb1c8a449474d8c65bd036557ca">
     <xsd:element name="properties">
@@ -4886,32 +4901,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21658938-80E1-42BC-AC12-1DA629B8A314}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECC0E455-C2DA-448A-8C29-80D30983133E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -4926,9 +4919,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECC0E455-C2DA-448A-8C29-80D30983133E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21658938-80E1-42BC-AC12-1DA629B8A314}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>